<commit_message>
Popis tvých změn (např. Oprava chyby v zobrazení tabulky)
</commit_message>
<xml_diff>
--- a/excel/Hodiny_Cap.xlsx
+++ b/excel/Hodiny_Cap.xlsx
@@ -1835,7 +1835,7 @@
       </c>
       <c r="C9" s="29" t="n"/>
       <c r="D9" s="26" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E9" s="27" t="n"/>
       <c r="F9" s="28" t="n"/>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="C10" s="25" t="n"/>
       <c r="D10" s="26" t="n">
-        <v>100</v>
+        <v>310</v>
       </c>
       <c r="E10" s="30" t="n"/>
       <c r="F10" s="28" t="n"/>
@@ -3059,8 +3059,8 @@
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="L18:M18"/>
-    <mergeCell ref="H6:I6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="J5:K5"/>
@@ -4142,8 +4142,8 @@
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="L18:M18"/>
-    <mergeCell ref="H6:I6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="J5:K5"/>
@@ -5216,8 +5216,8 @@
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="L18:M18"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="J5:K5"/>
@@ -5565,10 +5565,26 @@
           <t>17:00</t>
         </is>
       </c>
-      <c r="D7" s="41" t="n"/>
-      <c r="E7" s="41" t="n"/>
-      <c r="F7" s="41" t="n"/>
-      <c r="G7" s="41" t="n"/>
+      <c r="D7" s="41" t="inlineStr">
+        <is>
+          <t>07:30</t>
+        </is>
+      </c>
+      <c r="E7" s="41" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="F7" s="41" t="inlineStr">
+        <is>
+          <t>07:30</t>
+        </is>
+      </c>
+      <c r="G7" s="41" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
       <c r="H7" s="41" t="n"/>
       <c r="I7" s="41" t="n"/>
       <c r="J7" s="41" t="n"/>
@@ -5591,9 +5607,13 @@
         <v>8.5</v>
       </c>
       <c r="C8" s="91" t="n"/>
-      <c r="D8" s="90" t="n"/>
+      <c r="D8" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E8" s="91" t="n"/>
-      <c r="F8" s="90" t="n"/>
+      <c r="F8" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="G8" s="91" t="n"/>
       <c r="H8" s="90" t="n"/>
       <c r="I8" s="91" t="n"/>
@@ -5620,9 +5640,13 @@
         <v>8.5</v>
       </c>
       <c r="C9" s="91" t="n"/>
-      <c r="D9" s="90" t="n"/>
+      <c r="D9" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E9" s="91" t="n"/>
-      <c r="F9" s="90" t="n"/>
+      <c r="F9" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="G9" s="91" t="n"/>
       <c r="H9" s="90" t="n"/>
       <c r="I9" s="91" t="n"/>
@@ -5649,9 +5673,13 @@
         <v>8.5</v>
       </c>
       <c r="C10" s="91" t="n"/>
-      <c r="D10" s="90" t="n"/>
+      <c r="D10" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E10" s="91" t="n"/>
-      <c r="F10" s="90" t="n"/>
+      <c r="F10" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="G10" s="91" t="n"/>
       <c r="H10" s="90" t="n"/>
       <c r="I10" s="91" t="n"/>
@@ -5678,9 +5706,13 @@
         <v>8.5</v>
       </c>
       <c r="C11" s="91" t="n"/>
-      <c r="D11" s="90" t="n"/>
+      <c r="D11" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="E11" s="91" t="n"/>
-      <c r="F11" s="90" t="n"/>
+      <c r="F11" s="90" t="n">
+        <v>8.5</v>
+      </c>
       <c r="G11" s="91" t="n"/>
       <c r="H11" s="90" t="n"/>
       <c r="I11" s="91" t="n"/>
@@ -6182,11 +6214,21 @@
           <t>2024-12-09</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2024-12-10</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>2024-12-11</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="128">
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="L18:M18"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="J5:K5"/>

</xml_diff>

<commit_message>
Complete dynamic Excel configuration integration - full end-to-end working
Co-authored-by: CowleyCZE <159197257+CowleyCZE@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/excel/Hodiny_Cap.xlsx
+++ b/excel/Hodiny_Cap.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Zálohy" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Týden" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Týden 34" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +18,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="HH:MM"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="166" formatCode="DD.MM.YYYY"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +52,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -465,4 +473,113 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A7:E80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7">
+      <c r="D7" s="1" t="n">
+        <v>0.2916666666666667</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Čáp Jakub</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Horčička Jiří</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hromý Erik</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Kužel Andrej</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mlynář Roman</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Nastoupil Ladislav</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Winkler Jan</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Štrauf Daniel</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="D80" s="3" t="n">
+        <v>45888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor file upload handling to use in-memory bytes and improve merged cell management in Excel sheets; update last archived week in settings and add unit test for in-memory file upload verification.
</commit_message>
<xml_diff>
--- a/excel/Hodiny_Cap.xlsx
+++ b/excel/Hodiny_Cap.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Týden" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Zálohy" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Týden 34" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Zálohy" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Týden" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,10 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="HH:MM"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="166" formatCode="DD.MM.YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD.MM.YYYY"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -56,7 +54,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,24 +420,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="B80:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -475,111 +455,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A7:M80"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="7">
-      <c r="L7" s="1" t="n">
-        <v>0.2916666666666667</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Čáp Jakub</t>
-        </is>
-      </c>
-      <c r="M9" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Horčička Jiří</t>
-        </is>
-      </c>
-      <c r="M10" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Hromý Erik</t>
-        </is>
-      </c>
-      <c r="M11" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Kužel Andrej</t>
-        </is>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Mlynář Roman</t>
-        </is>
-      </c>
-      <c r="M13" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Nastoupil Ladislav</t>
-        </is>
-      </c>
-      <c r="M14" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Winkler Jan</t>
-        </is>
-      </c>
-      <c r="M15" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Štrauf Daniel</t>
-        </is>
-      </c>
-      <c r="M16" s="2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="L80" s="3" t="n">
-        <v>45892</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>